<commit_message>
about to write a doc
</commit_message>
<xml_diff>
--- a/ontologies/turbo_obib_ontodog_template.xlsx
+++ b/ontologies/turbo_obib_ontodog_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4401" uniqueCount="3737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4421" uniqueCount="3737">
   <si>
     <t>Source ontology term IRI</t>
   </si>
@@ -11588,10 +11588,10 @@
   <dimension ref="A1:E1721"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1109" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1299" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1140" sqref="D1140"/>
+      <selection pane="bottomRight" activeCell="A1324" sqref="A1324:XFD1324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -14237,6 +14237,9 @@
       <c r="B312" s="2" t="s">
         <v>2370</v>
       </c>
+      <c r="C312" s="2" t="s">
+        <v>3736</v>
+      </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="2" t="s">
@@ -18082,7 +18085,7 @@
         <v>3423</v>
       </c>
     </row>
-    <row r="753" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="753" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A753" s="2" t="s">
         <v>3016</v>
       </c>
@@ -18090,47 +18093,62 @@
         <v>3017</v>
       </c>
     </row>
-    <row r="754" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="754" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A754" s="2" t="s">
         <v>2335</v>
       </c>
       <c r="B754" s="2" t="s">
         <v>2336</v>
       </c>
-    </row>
-    <row r="755" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C754" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="755" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A755" s="2" t="s">
         <v>2337</v>
       </c>
       <c r="B755" s="2" t="s">
         <v>2338</v>
       </c>
-    </row>
-    <row r="756" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C755" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="756" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A756" s="2" t="s">
         <v>2339</v>
       </c>
       <c r="B756" s="2" t="s">
         <v>2340</v>
       </c>
-    </row>
-    <row r="757" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C756" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="757" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A757" s="2" t="s">
         <v>2341</v>
       </c>
       <c r="B757" s="2" t="s">
         <v>2342</v>
       </c>
-    </row>
-    <row r="758" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C757" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="758" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A758" s="2" t="s">
         <v>2343</v>
       </c>
       <c r="B758" s="2" t="s">
         <v>2344</v>
       </c>
-    </row>
-    <row r="759" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C758" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="759" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A759" s="2" t="s">
         <v>1507</v>
       </c>
@@ -18138,7 +18156,7 @@
         <v>1508</v>
       </c>
     </row>
-    <row r="760" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="760" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A760" s="2" t="s">
         <v>101</v>
       </c>
@@ -18146,7 +18164,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="761" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="761" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A761" s="2" t="s">
         <v>103</v>
       </c>
@@ -18154,7 +18172,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="762" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="762" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A762" s="2" t="s">
         <v>2505</v>
       </c>
@@ -18162,7 +18180,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="763" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="763" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A763" s="2" t="s">
         <v>2509</v>
       </c>
@@ -18170,7 +18188,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="764" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="764" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A764" s="2" t="s">
         <v>2511</v>
       </c>
@@ -18178,7 +18196,7 @@
         <v>2512</v>
       </c>
     </row>
-    <row r="765" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="765" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A765" s="2" t="s">
         <v>2279</v>
       </c>
@@ -18186,7 +18204,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="766" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="766" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A766" s="2" t="s">
         <v>2513</v>
       </c>
@@ -18194,7 +18212,7 @@
         <v>2514</v>
       </c>
     </row>
-    <row r="767" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="767" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A767" s="2" t="s">
         <v>2281</v>
       </c>
@@ -18202,7 +18220,7 @@
         <v>2282</v>
       </c>
     </row>
-    <row r="768" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="768" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A768" s="2" t="s">
         <v>639</v>
       </c>
@@ -18961,6 +18979,9 @@
       <c r="B856" s="2" t="s">
         <v>2372</v>
       </c>
+      <c r="C856" s="2" t="s">
+        <v>3736</v>
+      </c>
     </row>
     <row r="857" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A857" s="2" t="s">
@@ -18969,6 +18990,9 @@
       <c r="B857" s="2" t="s">
         <v>2374</v>
       </c>
+      <c r="C857" s="2" t="s">
+        <v>3736</v>
+      </c>
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A858" s="2" t="s">
@@ -21817,7 +21841,7 @@
         <v>3736</v>
       </c>
     </row>
-    <row r="1185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1185" s="2" t="s">
         <v>2461</v>
       </c>
@@ -21825,7 +21849,7 @@
         <v>2462</v>
       </c>
     </row>
-    <row r="1186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1186" s="2" t="s">
         <v>1761</v>
       </c>
@@ -21833,39 +21857,51 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="1187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1187" s="2" t="s">
         <v>2361</v>
       </c>
       <c r="B1187" s="2" t="s">
         <v>2362</v>
       </c>
-    </row>
-    <row r="1188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1187" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1188" s="2" t="s">
         <v>2365</v>
       </c>
       <c r="B1188" s="2" t="s">
         <v>2366</v>
       </c>
-    </row>
-    <row r="1189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1188" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1189" s="2" t="s">
         <v>2363</v>
       </c>
       <c r="B1189" s="2" t="s">
         <v>2364</v>
       </c>
-    </row>
-    <row r="1190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1189" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1190" s="2" t="s">
         <v>2367</v>
       </c>
       <c r="B1190" s="2" t="s">
         <v>2368</v>
       </c>
-    </row>
-    <row r="1191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1190" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1191" s="2" t="s">
         <v>589</v>
       </c>
@@ -21873,71 +21909,95 @@
         <v>590</v>
       </c>
     </row>
-    <row r="1192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1192" s="2" t="s">
         <v>2353</v>
       </c>
       <c r="B1192" s="2" t="s">
         <v>2354</v>
       </c>
-    </row>
-    <row r="1193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1192" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1193" s="2" t="s">
         <v>2357</v>
       </c>
       <c r="B1193" s="2" t="s">
         <v>2358</v>
       </c>
-    </row>
-    <row r="1194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1193" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1194" s="2" t="s">
         <v>2355</v>
       </c>
       <c r="B1194" s="2" t="s">
         <v>2356</v>
       </c>
-    </row>
-    <row r="1195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1194" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1195" s="2" t="s">
         <v>2359</v>
       </c>
       <c r="B1195" s="2" t="s">
         <v>2360</v>
       </c>
-    </row>
-    <row r="1196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1195" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1196" s="2" t="s">
         <v>2345</v>
       </c>
       <c r="B1196" s="2" t="s">
         <v>2346</v>
       </c>
-    </row>
-    <row r="1197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1196" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1197" s="2" t="s">
         <v>2349</v>
       </c>
       <c r="B1197" s="2" t="s">
         <v>2350</v>
       </c>
-    </row>
-    <row r="1198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1197" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1198" s="2" t="s">
         <v>2347</v>
       </c>
       <c r="B1198" s="2" t="s">
         <v>2348</v>
       </c>
-    </row>
-    <row r="1199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1198" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1199" s="2" t="s">
         <v>2351</v>
       </c>
       <c r="B1199" s="2" t="s">
         <v>2352</v>
       </c>
-    </row>
-    <row r="1200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1199" s="2" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1200" s="2" t="s">
         <v>1497</v>
       </c>
@@ -22865,9 +22925,6 @@
       <c r="B1308" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="C1308" s="2" t="s">
-        <v>3736</v>
-      </c>
     </row>
     <row r="1309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1309" s="2" t="s">
@@ -23013,6 +23070,9 @@
       </c>
       <c r="B1324" s="2" t="s">
         <v>3009</v>
+      </c>
+      <c r="C1324" s="2" t="s">
+        <v>3736</v>
       </c>
     </row>
     <row r="1325" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>